<commit_message>
make skeleton of starter scene
</commit_message>
<xml_diff>
--- a/Assets/Sprites/source.xlsx
+++ b/Assets/Sprites/source.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -44,7 +44,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +55,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -83,8 +91,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -404,28 +415,30 @@
   <dimension ref="B1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.375" customWidth="1"/>
-    <col min="3" max="3" width="51.125" customWidth="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="21.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="51.125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>